<commit_message>
update database with better record
</commit_message>
<xml_diff>
--- a/project2/tetris3D/sample.xlsx
+++ b/project2/tetris3D/sample.xlsx
@@ -1,20 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<s:workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:s="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <s:workbookPr/>
-  <s:bookViews>
-    <s:workbookView activeTab="0"/>
-  </s:bookViews>
-  <s:sheets>
-    <s:sheet name="score sheet 1" sheetId="1" r:id="rId1"/>
-  </s:sheets>
-  <s:definedNames/>
-  <s:calcPr calcId="124519" fullCalcOnLoad="1"/>
-</s:workbook>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Score-Management-Subsystem\project2\tetris3D\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <bookViews>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19140" windowHeight="7665"/>
+  </bookViews>
+  <sheets>
+    <sheet name="score sheet 1" sheetId="1" r:id="rId1"/>
+  </sheets>
+  <calcPr calcId="0"/>
+</workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
   <si>
     <t>浙江大学课程考试成绩记录表</t>
   </si>
@@ -28,6 +33,9 @@
     <t>课程编号</t>
   </si>
   <si>
+    <t>0000000001</t>
+  </si>
+  <si>
     <t>学号</t>
   </si>
   <si>
@@ -38,9 +46,6 @@
   </si>
   <si>
     <t>备注</t>
-  </si>
-  <si>
-    <t>0000000001</t>
   </si>
   <si>
     <t>zhazha</t>
@@ -67,20 +72,26 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
-      <name val="Calibri"/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -96,19 +107,28 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+  <cellXfs count="3">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -396,89 +416,111 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:s="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <s:sheetPr>
-    <s:outlinePr summaryBelow="1" summaryRight="1"/>
-    <s:pageSetUpPr/>
-  </s:sheetPr>
-  <dimension ref="A1:E8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:5">
-      <c r="A2" t="s">
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A2" s="2"/>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A3" t="s">
         <v>1</v>
       </c>
-      <c r="B2" t="s"/>
-      <c r="C2" t="s">
+      <c r="C3" t="s">
         <v>2</v>
       </c>
-      <c r="D2" t="s"/>
-      <c r="E2" t="s">
+      <c r="E3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:5"/>
-    <row r="4" spans="1:5">
-      <c r="A4" t="s">
+      <c r="F3" t="s">
         <v>4</v>
       </c>
-      <c r="B4" t="s">
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A5" t="s">
         <v>5</v>
       </c>
-      <c r="C4" t="s">
+      <c r="B5" t="s">
         <v>6</v>
       </c>
-      <c r="D4" t="s">
+      <c r="C5" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="5" spans="1:5">
-      <c r="A5" t="s">
+      <c r="D5" t="s">
         <v>8</v>
       </c>
-      <c r="B5" t="s">
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="6" spans="1:5">
-      <c r="A6" t="s">
+      <c r="C6">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A7" t="s">
         <v>10</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B7" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="7" spans="1:5">
-      <c r="A7" t="s">
+      <c r="C7">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A8" t="s">
         <v>12</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B8" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="8" spans="1:5">
-      <c r="A8" t="s">
+      <c r="C8">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A9" t="s">
         <v>14</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B9" t="s">
         <v>15</v>
+      </c>
+      <c r="C9">
+        <v>59</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:F2"/>
   </mergeCells>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
-  <pageSetup fitToWidth="1"/>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>